<commit_message>
adding hot water usage disturbances
</commit_message>
<xml_diff>
--- a/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
+++ b/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
@@ -130,8 +130,8 @@
   </sheetPr>
   <dimension ref="A1:B722"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A694" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A722" activeCellId="0" sqref="722:1297"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A327" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C348" activeCellId="0" sqref="C348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,787 +471,787 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <f aca="false">A37+TIME(0,10,0)</f>
         <v>43221.25</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <f aca="false">A38+TIME(0,10,0)</f>
         <v>43221.2569444445</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <f aca="false">A39+TIME(0,10,0)</f>
         <v>43221.2638888889</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <f aca="false">A40+TIME(0,10,0)</f>
         <v>43221.2708333334</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <f aca="false">A41+TIME(0,10,0)</f>
         <v>43221.2777777778</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <f aca="false">A42+TIME(0,10,0)</f>
         <v>43221.2847222223</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <f aca="false">A43+TIME(0,10,0)</f>
         <v>43221.2916666667</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <f aca="false">A44+TIME(0,10,0)</f>
         <v>43221.2986111111</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <f aca="false">A45+TIME(0,10,0)</f>
         <v>43221.3055555556</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <f aca="false">A46+TIME(0,10,0)</f>
         <v>43221.3125</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <f aca="false">A47+TIME(0,10,0)</f>
         <v>43221.3194444445</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <f aca="false">A48+TIME(0,10,0)</f>
         <v>43221.3263888889</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <f aca="false">A49+TIME(0,10,0)</f>
         <v>43221.3333333334</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <f aca="false">A50+TIME(0,10,0)</f>
         <v>43221.3402777778</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <f aca="false">A51+TIME(0,10,0)</f>
         <v>43221.3472222223</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <f aca="false">A52+TIME(0,10,0)</f>
         <v>43221.3541666667</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <f aca="false">A53+TIME(0,10,0)</f>
         <v>43221.3611111112</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <f aca="false">A54+TIME(0,10,0)</f>
         <v>43221.3680555556</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <f aca="false">A55+TIME(0,10,0)</f>
         <v>43221.375</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <f aca="false">A56+TIME(0,10,0)</f>
         <v>43221.3819444445</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <f aca="false">A57+TIME(0,10,0)</f>
         <v>43221.3888888889</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <f aca="false">A58+TIME(0,10,0)</f>
         <v>43221.3958333334</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <f aca="false">A59+TIME(0,10,0)</f>
         <v>43221.4027777778</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <f aca="false">A60+TIME(0,10,0)</f>
         <v>43221.4097222223</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <f aca="false">A61+TIME(0,10,0)</f>
         <v>43221.4166666667</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <f aca="false">A62+TIME(0,10,0)</f>
         <v>43221.4236111112</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <f aca="false">A63+TIME(0,10,0)</f>
         <v>43221.4305555556</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <f aca="false">A64+TIME(0,10,0)</f>
         <v>43221.4375000001</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <f aca="false">A65+TIME(0,10,0)</f>
         <v>43221.4444444445</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <f aca="false">A66+TIME(0,10,0)</f>
         <v>43221.4513888889</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <f aca="false">A67+TIME(0,10,0)</f>
         <v>43221.4583333334</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <f aca="false">A68+TIME(0,10,0)</f>
         <v>43221.4652777778</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <f aca="false">A69+TIME(0,10,0)</f>
         <v>43221.4722222223</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <f aca="false">A70+TIME(0,10,0)</f>
         <v>43221.4791666667</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <f aca="false">A71+TIME(0,10,0)</f>
         <v>43221.4861111112</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <f aca="false">A72+TIME(0,10,0)</f>
         <v>43221.4930555556</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
         <f aca="false">A73+TIME(0,10,0)</f>
         <v>43221.5000000001</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <f aca="false">A74+TIME(0,10,0)</f>
         <v>43221.5069444445</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <f aca="false">A75+TIME(0,10,0)</f>
         <v>43221.513888889</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <f aca="false">A76+TIME(0,10,0)</f>
         <v>43221.5208333334</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <f aca="false">A77+TIME(0,10,0)</f>
         <v>43221.5277777778</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <f aca="false">A78+TIME(0,10,0)</f>
         <v>43221.5347222223</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
         <f aca="false">A79+TIME(0,10,0)</f>
         <v>43221.5416666667</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
         <f aca="false">A80+TIME(0,10,0)</f>
         <v>43221.5486111112</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
         <f aca="false">A81+TIME(0,10,0)</f>
         <v>43221.5555555556</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
         <f aca="false">A82+TIME(0,10,0)</f>
         <v>43221.5625000001</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
         <f aca="false">A83+TIME(0,10,0)</f>
         <v>43221.5694444445</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
         <f aca="false">A84+TIME(0,10,0)</f>
         <v>43221.576388889</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
         <f aca="false">A85+TIME(0,10,0)</f>
         <v>43221.5833333334</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
         <f aca="false">A86+TIME(0,10,0)</f>
         <v>43221.5902777778</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
         <f aca="false">A87+TIME(0,10,0)</f>
         <v>43221.5972222223</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
         <f aca="false">A88+TIME(0,10,0)</f>
         <v>43221.6041666667</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
         <f aca="false">A89+TIME(0,10,0)</f>
         <v>43221.6111111112</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
         <f aca="false">A90+TIME(0,10,0)</f>
         <v>43221.6180555556</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
         <f aca="false">A91+TIME(0,10,0)</f>
         <v>43221.6250000001</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
         <f aca="false">A92+TIME(0,10,0)</f>
         <v>43221.6319444445</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
         <f aca="false">A93+TIME(0,10,0)</f>
         <v>43221.638888889</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
         <f aca="false">A94+TIME(0,10,0)</f>
         <v>43221.6458333334</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
         <f aca="false">A95+TIME(0,10,0)</f>
         <v>43221.6527777779</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
         <f aca="false">A96+TIME(0,10,0)</f>
         <v>43221.6597222223</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
         <f aca="false">A97+TIME(0,10,0)</f>
         <v>43221.6666666667</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
         <f aca="false">A98+TIME(0,10,0)</f>
         <v>43221.6736111112</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
         <f aca="false">A99+TIME(0,10,0)</f>
         <v>43221.6805555556</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
         <f aca="false">A100+TIME(0,10,0)</f>
         <v>43221.6875000001</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
         <f aca="false">A101+TIME(0,10,0)</f>
         <v>43221.6944444445</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
         <f aca="false">A102+TIME(0,10,0)</f>
         <v>43221.701388889</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
         <f aca="false">A103+TIME(0,10,0)</f>
         <v>43221.7083333334</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
         <f aca="false">A104+TIME(0,10,0)</f>
         <v>43221.7152777779</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
         <f aca="false">A105+TIME(0,10,0)</f>
         <v>43221.7222222223</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
         <f aca="false">A106+TIME(0,10,0)</f>
         <v>43221.7291666668</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
         <f aca="false">A107+TIME(0,10,0)</f>
         <v>43221.7361111112</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
         <f aca="false">A108+TIME(0,10,0)</f>
         <v>43221.7430555556</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
         <f aca="false">A109+TIME(0,10,0)</f>
         <v>43221.7500000001</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
         <f aca="false">A110+TIME(0,10,0)</f>
         <v>43221.7569444445</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
         <f aca="false">A111+TIME(0,10,0)</f>
         <v>43221.763888889</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
         <f aca="false">A112+TIME(0,10,0)</f>
         <v>43221.7708333334</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
         <f aca="false">A113+TIME(0,10,0)</f>
         <v>43221.7777777779</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
         <f aca="false">A114+TIME(0,10,0)</f>
         <v>43221.7847222223</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <f aca="false">A115+TIME(0,10,0)</f>
         <v>43221.7916666668</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
         <f aca="false">A116+TIME(0,10,0)</f>
         <v>43221.7986111112</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
         <f aca="false">A117+TIME(0,10,0)</f>
         <v>43221.8055555556</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
         <f aca="false">A118+TIME(0,10,0)</f>
         <v>43221.8125000001</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
         <f aca="false">A119+TIME(0,10,0)</f>
         <v>43221.8194444445</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <f aca="false">A120+TIME(0,10,0)</f>
         <v>43221.826388889</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
         <f aca="false">A121+TIME(0,10,0)</f>
         <v>43221.8333333334</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <f aca="false">A122+TIME(0,10,0)</f>
         <v>43221.8402777779</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
         <f aca="false">A123+TIME(0,10,0)</f>
         <v>43221.8472222223</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,7 +1260,7 @@
         <v>43221.8541666668</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1269,7 @@
         <v>43221.8611111112</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1278,7 @@
         <v>43221.8680555557</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,7 +1287,7 @@
         <v>43221.8750000001</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1296,43 +1296,43 @@
         <v>43221.8819444446</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
         <f aca="false">A129+TIME(0,10,0)</f>
         <v>43221.888888889</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
         <f aca="false">A130+TIME(0,10,0)</f>
         <v>43221.8958333334</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
         <f aca="false">A131+TIME(0,10,0)</f>
         <v>43221.9027777779</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
         <f aca="false">A132+TIME(0,10,0)</f>
         <v>43221.9097222223</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1773,7 @@
         <v>43222.2500000001</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,7 +1782,7 @@
         <v>43222.2569444446</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1791,7 @@
         <v>43222.263888889</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,7 +1800,7 @@
         <v>43222.2708333335</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,7 +1809,7 @@
         <v>43222.2777777779</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1818,7 @@
         <v>43222.2847222224</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1827,7 @@
         <v>43222.2916666668</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>43222.2986111113</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1845,7 @@
         <v>43222.3055555557</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
         <v>43222.3125000002</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1863,7 @@
         <v>43222.3194444446</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>43222.326388889</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1881,7 @@
         <v>43222.3333333335</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1890,7 @@
         <v>43222.3402777779</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,7 +1899,7 @@
         <v>43222.3472222224</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1908,7 @@
         <v>43222.3541666668</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +1917,7 @@
         <v>43222.3611111113</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1926,7 @@
         <v>43222.3680555557</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
         <v>43222.3750000002</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1944,7 @@
         <v>43222.3819444446</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,7 +1953,7 @@
         <v>43222.3888888891</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,7 +1962,7 @@
         <v>43222.3958333335</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>43222.4027777779</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1980,7 @@
         <v>43222.4097222224</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1989,7 @@
         <v>43222.4166666668</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +1998,7 @@
         <v>43222.4236111113</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,7 +2007,7 @@
         <v>43222.4305555557</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2016,7 @@
         <v>43222.4375000002</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2025,7 @@
         <v>43222.4444444446</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2034,7 @@
         <v>43222.4513888891</v>
       </c>
       <c r="B211" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2043,7 @@
         <v>43222.4583333335</v>
       </c>
       <c r="B212" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,7 +2052,7 @@
         <v>43222.4652777779</v>
       </c>
       <c r="B213" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2061,7 @@
         <v>43222.4722222224</v>
       </c>
       <c r="B214" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>43222.4791666668</v>
       </c>
       <c r="B215" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2079,7 @@
         <v>43222.4861111113</v>
       </c>
       <c r="B216" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2088,7 @@
         <v>43222.4930555557</v>
       </c>
       <c r="B217" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,7 +2097,7 @@
         <v>43222.5000000002</v>
       </c>
       <c r="B218" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2106,7 @@
         <v>43222.5069444446</v>
       </c>
       <c r="B219" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +2115,7 @@
         <v>43222.5138888891</v>
       </c>
       <c r="B220" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2124,7 @@
         <v>43222.5208333335</v>
       </c>
       <c r="B221" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2133,7 @@
         <v>43222.527777778</v>
       </c>
       <c r="B222" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2142,7 @@
         <v>43222.5347222224</v>
       </c>
       <c r="B223" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,7 +2151,7 @@
         <v>43222.5416666669</v>
       </c>
       <c r="B224" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>43222.5486111113</v>
       </c>
       <c r="B225" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2169,7 @@
         <v>43222.5555555557</v>
       </c>
       <c r="B226" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2178,7 @@
         <v>43222.5625000002</v>
       </c>
       <c r="B227" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2187,7 @@
         <v>43222.5694444446</v>
       </c>
       <c r="B228" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2196,7 @@
         <v>43222.5763888891</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2205,7 @@
         <v>43222.5833333335</v>
       </c>
       <c r="B230" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,7 +2214,7 @@
         <v>43222.590277778</v>
       </c>
       <c r="B231" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2223,7 @@
         <v>43222.5972222224</v>
       </c>
       <c r="B232" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2232,7 @@
         <v>43222.6041666669</v>
       </c>
       <c r="B233" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,7 +2241,7 @@
         <v>43222.6111111113</v>
       </c>
       <c r="B234" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2250,7 @@
         <v>43222.6180555557</v>
       </c>
       <c r="B235" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,7 +2259,7 @@
         <v>43222.6250000002</v>
       </c>
       <c r="B236" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2268,7 @@
         <v>43222.6319444446</v>
       </c>
       <c r="B237" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2277,7 @@
         <v>43222.6388888891</v>
       </c>
       <c r="B238" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>43222.6458333335</v>
       </c>
       <c r="B239" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,7 +2295,7 @@
         <v>43222.652777778</v>
       </c>
       <c r="B240" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,7 +2304,7 @@
         <v>43222.6597222224</v>
       </c>
       <c r="B241" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2313,7 @@
         <v>43222.6666666669</v>
       </c>
       <c r="B242" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2322,7 @@
         <v>43222.6736111113</v>
       </c>
       <c r="B243" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,7 +2331,7 @@
         <v>43222.6805555558</v>
       </c>
       <c r="B244" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2340,7 @@
         <v>43222.6875000002</v>
       </c>
       <c r="B245" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2349,7 @@
         <v>43222.6944444446</v>
       </c>
       <c r="B246" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,7 +2358,7 @@
         <v>43222.7013888891</v>
       </c>
       <c r="B247" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,7 +2367,7 @@
         <v>43222.7083333335</v>
       </c>
       <c r="B248" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,7 +2376,7 @@
         <v>43222.715277778</v>
       </c>
       <c r="B249" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>43222.7222222224</v>
       </c>
       <c r="B250" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2394,7 @@
         <v>43222.7291666669</v>
       </c>
       <c r="B251" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2403,7 @@
         <v>43222.7361111113</v>
       </c>
       <c r="B252" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,7 +2412,7 @@
         <v>43222.7430555558</v>
       </c>
       <c r="B253" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2421,7 @@
         <v>43222.7500000002</v>
       </c>
       <c r="B254" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2430,7 @@
         <v>43222.7569444447</v>
       </c>
       <c r="B255" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,7 +2439,7 @@
         <v>43222.7638888891</v>
       </c>
       <c r="B256" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,7 +2448,7 @@
         <v>43222.7708333335</v>
       </c>
       <c r="B257" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2457,7 @@
         <v>43222.777777778</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2466,7 @@
         <v>43222.7847222224</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2475,7 @@
         <v>43222.7916666669</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>43222.7986111113</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2493,7 @@
         <v>43222.8055555558</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2502,7 @@
         <v>43222.8125000002</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,7 +2511,7 @@
         <v>43222.8194444447</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2520,7 @@
         <v>43222.8263888891</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,7 +2529,7 @@
         <v>43222.8333333335</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,7 +2538,7 @@
         <v>43222.840277778</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2547,7 @@
         <v>43222.8472222224</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,7 +2556,7 @@
         <v>43222.8541666669</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2565,7 @@
         <v>43222.8611111113</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,7 +2574,7 @@
         <v>43222.8680555558</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>43222.8750000002</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2592,7 @@
         <v>43222.8819444447</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,7 +2601,7 @@
         <v>43222.8888888891</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2610,7 @@
         <v>43222.8958333336</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2619,7 @@
         <v>43222.902777778</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,7 +2628,7 @@
         <v>43222.9097222225</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,7 +3069,7 @@
         <v>43223.2500000003</v>
       </c>
       <c r="B326" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,7 +3078,7 @@
         <v>43223.2569444447</v>
       </c>
       <c r="B327" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,7 +3087,7 @@
         <v>43223.2638888892</v>
       </c>
       <c r="B328" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,7 +3096,7 @@
         <v>43223.2708333336</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,7 +3105,7 @@
         <v>43223.277777778</v>
       </c>
       <c r="B330" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,7 +3114,7 @@
         <v>43223.2847222225</v>
       </c>
       <c r="B331" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,7 +3123,7 @@
         <v>43223.2916666669</v>
       </c>
       <c r="B332" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3132,7 @@
         <v>43223.2986111114</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,7 +3141,7 @@
         <v>43223.3055555558</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,7 +3150,7 @@
         <v>43223.3125000003</v>
       </c>
       <c r="B335" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,7 +3159,7 @@
         <v>43223.3194444447</v>
       </c>
       <c r="B336" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3168,7 @@
         <v>43223.3263888892</v>
       </c>
       <c r="B337" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,7 +3177,7 @@
         <v>43223.3333333336</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3186,7 @@
         <v>43223.340277778</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,7 +3195,7 @@
         <v>43223.3472222225</v>
       </c>
       <c r="B340" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,7 +3204,7 @@
         <v>43223.3541666669</v>
       </c>
       <c r="B341" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,7 +3213,7 @@
         <v>43223.3611111114</v>
       </c>
       <c r="B342" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3222,7 +3222,7 @@
         <v>43223.3680555558</v>
       </c>
       <c r="B343" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,7 +3231,7 @@
         <v>43223.3750000003</v>
       </c>
       <c r="B344" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,7 +3240,7 @@
         <v>43223.3819444447</v>
       </c>
       <c r="B345" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,7 +3249,7 @@
         <v>43223.3888888892</v>
       </c>
       <c r="B346" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,7 +3258,7 @@
         <v>43223.3958333336</v>
       </c>
       <c r="B347" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,7 +3267,7 @@
         <v>43223.4027777781</v>
       </c>
       <c r="B348" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,7 +3276,7 @@
         <v>43223.4097222225</v>
       </c>
       <c r="B349" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3285,7 @@
         <v>43223.416666667</v>
       </c>
       <c r="B350" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3294,7 +3294,7 @@
         <v>43223.4236111114</v>
       </c>
       <c r="B351" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,7 +3303,7 @@
         <v>43223.4305555558</v>
       </c>
       <c r="B352" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,7 +3312,7 @@
         <v>43223.4375000003</v>
       </c>
       <c r="B353" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,7 +3321,7 @@
         <v>43223.4444444447</v>
       </c>
       <c r="B354" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,7 +3330,7 @@
         <v>43223.4513888892</v>
       </c>
       <c r="B355" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3339,7 @@
         <v>43223.4583333336</v>
       </c>
       <c r="B356" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3348,7 +3348,7 @@
         <v>43223.4652777781</v>
       </c>
       <c r="B357" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3357,7 @@
         <v>43223.4722222225</v>
       </c>
       <c r="B358" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,7 +3366,7 @@
         <v>43223.479166667</v>
       </c>
       <c r="B359" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,7 +3375,7 @@
         <v>43223.4861111114</v>
       </c>
       <c r="B360" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3384,7 @@
         <v>43223.4930555558</v>
       </c>
       <c r="B361" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,7 +3393,7 @@
         <v>43223.5000000003</v>
       </c>
       <c r="B362" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,7 +3402,7 @@
         <v>43223.5069444447</v>
       </c>
       <c r="B363" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,7 +3411,7 @@
         <v>43223.5138888892</v>
       </c>
       <c r="B364" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,7 +3420,7 @@
         <v>43223.5208333336</v>
       </c>
       <c r="B365" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,7 +3429,7 @@
         <v>43223.5277777781</v>
       </c>
       <c r="B366" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3438,7 +3438,7 @@
         <v>43223.5347222225</v>
       </c>
       <c r="B367" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3447,7 @@
         <v>43223.541666667</v>
       </c>
       <c r="B368" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3456,7 @@
         <v>43223.5486111114</v>
       </c>
       <c r="B369" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,7 +3465,7 @@
         <v>43223.5555555559</v>
       </c>
       <c r="B370" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,7 +3474,7 @@
         <v>43223.5625000003</v>
       </c>
       <c r="B371" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3483,7 @@
         <v>43223.5694444448</v>
       </c>
       <c r="B372" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3492,7 +3492,7 @@
         <v>43223.5763888892</v>
       </c>
       <c r="B373" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,7 +3501,7 @@
         <v>43223.5833333336</v>
       </c>
       <c r="B374" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3510,7 +3510,7 @@
         <v>43223.5902777781</v>
       </c>
       <c r="B375" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,7 +3519,7 @@
         <v>43223.5972222225</v>
       </c>
       <c r="B376" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3528,7 +3528,7 @@
         <v>43223.604166667</v>
       </c>
       <c r="B377" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,7 +3537,7 @@
         <v>43223.6111111114</v>
       </c>
       <c r="B378" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3546,7 @@
         <v>43223.6180555559</v>
       </c>
       <c r="B379" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,7 +3555,7 @@
         <v>43223.6250000003</v>
       </c>
       <c r="B380" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +3564,7 @@
         <v>43223.6319444448</v>
       </c>
       <c r="B381" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,7 +3573,7 @@
         <v>43223.6388888892</v>
       </c>
       <c r="B382" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3582,7 @@
         <v>43223.6458333336</v>
       </c>
       <c r="B383" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,7 +3591,7 @@
         <v>43223.6527777781</v>
       </c>
       <c r="B384" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,7 +3600,7 @@
         <v>43223.6597222225</v>
       </c>
       <c r="B385" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,7 +3609,7 @@
         <v>43223.666666667</v>
       </c>
       <c r="B386" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3618,7 @@
         <v>43223.6736111114</v>
       </c>
       <c r="B387" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,7 +3627,7 @@
         <v>43223.6805555559</v>
       </c>
       <c r="B388" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,7 +3636,7 @@
         <v>43223.6875000003</v>
       </c>
       <c r="B389" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,7 +3645,7 @@
         <v>43223.6944444448</v>
       </c>
       <c r="B390" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3654,7 +3654,7 @@
         <v>43223.7013888892</v>
       </c>
       <c r="B391" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3663,7 @@
         <v>43223.7083333337</v>
       </c>
       <c r="B392" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,7 +3672,7 @@
         <v>43223.7152777781</v>
       </c>
       <c r="B393" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,7 +3681,7 @@
         <v>43223.7222222225</v>
       </c>
       <c r="B394" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3690,7 +3690,7 @@
         <v>43223.729166667</v>
       </c>
       <c r="B395" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,7 +3699,7 @@
         <v>43223.7361111114</v>
       </c>
       <c r="B396" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,7 +3708,7 @@
         <v>43223.7430555559</v>
       </c>
       <c r="B397" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,7 +3717,7 @@
         <v>43223.7500000003</v>
       </c>
       <c r="B398" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3726,7 @@
         <v>43223.7569444448</v>
       </c>
       <c r="B399" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,7 +3735,7 @@
         <v>43223.7638888892</v>
       </c>
       <c r="B400" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,7 +3744,7 @@
         <v>43223.7708333337</v>
       </c>
       <c r="B401" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,7 +3753,7 @@
         <v>43223.7777777781</v>
       </c>
       <c r="B402" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3762,7 @@
         <v>43223.7847222226</v>
       </c>
       <c r="B403" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,7 +3771,7 @@
         <v>43223.791666667</v>
       </c>
       <c r="B404" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3780,7 +3780,7 @@
         <v>43223.7986111114</v>
       </c>
       <c r="B405" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,7 +3789,7 @@
         <v>43223.8055555559</v>
       </c>
       <c r="B406" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,7 +3798,7 @@
         <v>43223.8125000003</v>
       </c>
       <c r="B407" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,7 +3807,7 @@
         <v>43223.8194444448</v>
       </c>
       <c r="B408" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,7 +3816,7 @@
         <v>43223.8263888892</v>
       </c>
       <c r="B409" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,7 +3825,7 @@
         <v>43223.8333333337</v>
       </c>
       <c r="B410" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,7 +3834,7 @@
         <v>43223.8402777781</v>
       </c>
       <c r="B411" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3843,7 @@
         <v>43223.8472222226</v>
       </c>
       <c r="B412" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,7 +3852,7 @@
         <v>43223.854166667</v>
       </c>
       <c r="B413" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>43223.8611111114</v>
       </c>
       <c r="B414" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3870,7 +3870,7 @@
         <v>43223.8680555559</v>
       </c>
       <c r="B415" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,7 +3879,7 @@
         <v>43223.8750000003</v>
       </c>
       <c r="B416" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3888,7 +3888,7 @@
         <v>43223.8819444448</v>
       </c>
       <c r="B417" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,7 +3897,7 @@
         <v>43223.8888888892</v>
       </c>
       <c r="B418" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,7 +3906,7 @@
         <v>43223.8958333337</v>
       </c>
       <c r="B419" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3915,7 @@
         <v>43223.9027777781</v>
       </c>
       <c r="B420" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,7 +3924,7 @@
         <v>43223.9097222226</v>
       </c>
       <c r="B421" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4365,7 +4365,7 @@
         <v>43224.2500000004</v>
       </c>
       <c r="B470" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4374,7 @@
         <v>43224.2569444448</v>
       </c>
       <c r="B471" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4383,7 +4383,7 @@
         <v>43224.2638888893</v>
       </c>
       <c r="B472" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,7 +4392,7 @@
         <v>43224.2708333337</v>
       </c>
       <c r="B473" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4401,7 +4401,7 @@
         <v>43224.2777777782</v>
       </c>
       <c r="B474" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4410,7 @@
         <v>43224.2847222226</v>
       </c>
       <c r="B475" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,7 +4419,7 @@
         <v>43224.2916666671</v>
       </c>
       <c r="B476" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,7 +4428,7 @@
         <v>43224.2986111115</v>
       </c>
       <c r="B477" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,7 +4437,7 @@
         <v>43224.3055555559</v>
       </c>
       <c r="B478" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,7 +4446,7 @@
         <v>43224.3125000004</v>
       </c>
       <c r="B479" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4455,7 +4455,7 @@
         <v>43224.3194444448</v>
       </c>
       <c r="B480" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4464,7 @@
         <v>43224.3263888893</v>
       </c>
       <c r="B481" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,7 +4473,7 @@
         <v>43224.3333333337</v>
       </c>
       <c r="B482" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,7 +4482,7 @@
         <v>43224.3402777782</v>
       </c>
       <c r="B483" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4491,7 +4491,7 @@
         <v>43224.3472222226</v>
       </c>
       <c r="B484" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,7 +4500,7 @@
         <v>43224.3541666671</v>
       </c>
       <c r="B485" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4509,7 +4509,7 @@
         <v>43224.3611111115</v>
       </c>
       <c r="B486" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4518,7 @@
         <v>43224.3680555559</v>
       </c>
       <c r="B487" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,7 +4527,7 @@
         <v>43224.3750000004</v>
       </c>
       <c r="B488" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,7 @@
         <v>43224.3819444448</v>
       </c>
       <c r="B489" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4545,7 +4545,7 @@
         <v>43224.3888888893</v>
       </c>
       <c r="B490" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,7 +4554,7 @@
         <v>43224.3958333337</v>
       </c>
       <c r="B491" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4563,7 +4563,7 @@
         <v>43224.4027777782</v>
       </c>
       <c r="B492" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4572,7 +4572,7 @@
         <v>43224.4097222226</v>
       </c>
       <c r="B493" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4581,7 +4581,7 @@
         <v>43224.4166666671</v>
       </c>
       <c r="B494" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,7 +4590,7 @@
         <v>43224.4236111115</v>
       </c>
       <c r="B495" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,7 +4599,7 @@
         <v>43224.430555556</v>
       </c>
       <c r="B496" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,7 +4608,7 @@
         <v>43224.4375000004</v>
       </c>
       <c r="B497" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,7 +4617,7 @@
         <v>43224.4444444449</v>
       </c>
       <c r="B498" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4626,7 +4626,7 @@
         <v>43224.4513888893</v>
       </c>
       <c r="B499" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4635,7 +4635,7 @@
         <v>43224.4583333337</v>
       </c>
       <c r="B500" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4644,7 +4644,7 @@
         <v>43224.4652777782</v>
       </c>
       <c r="B501" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4653,7 +4653,7 @@
         <v>43224.4722222226</v>
       </c>
       <c r="B502" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4662,7 +4662,7 @@
         <v>43224.4791666671</v>
       </c>
       <c r="B503" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4671,7 +4671,7 @@
         <v>43224.4861111115</v>
       </c>
       <c r="B504" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4680,7 @@
         <v>43224.493055556</v>
       </c>
       <c r="B505" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4689,7 +4689,7 @@
         <v>43224.5000000004</v>
       </c>
       <c r="B506" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4698,7 +4698,7 @@
         <v>43224.5069444449</v>
       </c>
       <c r="B507" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,7 +4707,7 @@
         <v>43224.5138888893</v>
       </c>
       <c r="B508" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4716,7 +4716,7 @@
         <v>43224.5208333337</v>
       </c>
       <c r="B509" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,7 +4725,7 @@
         <v>43224.5277777782</v>
       </c>
       <c r="B510" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,7 +4734,7 @@
         <v>43224.5347222226</v>
       </c>
       <c r="B511" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4743,7 +4743,7 @@
         <v>43224.5416666671</v>
       </c>
       <c r="B512" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4752,7 +4752,7 @@
         <v>43224.5486111115</v>
       </c>
       <c r="B513" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4761,7 +4761,7 @@
         <v>43224.555555556</v>
       </c>
       <c r="B514" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,7 +4770,7 @@
         <v>43224.5625000004</v>
       </c>
       <c r="B515" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4779,7 +4779,7 @@
         <v>43224.5694444449</v>
       </c>
       <c r="B516" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4788,7 +4788,7 @@
         <v>43224.5763888893</v>
       </c>
       <c r="B517" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4797,7 @@
         <v>43224.5833333338</v>
       </c>
       <c r="B518" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4806,7 +4806,7 @@
         <v>43224.5902777782</v>
       </c>
       <c r="B519" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4815,7 +4815,7 @@
         <v>43224.5972222226</v>
       </c>
       <c r="B520" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4824,7 +4824,7 @@
         <v>43224.6041666671</v>
       </c>
       <c r="B521" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4833,7 @@
         <v>43224.6111111115</v>
       </c>
       <c r="B522" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,7 +4842,7 @@
         <v>43224.618055556</v>
       </c>
       <c r="B523" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,7 +4851,7 @@
         <v>43224.6250000004</v>
       </c>
       <c r="B524" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4860,7 +4860,7 @@
         <v>43224.6319444449</v>
       </c>
       <c r="B525" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4869,7 +4869,7 @@
         <v>43224.6388888893</v>
       </c>
       <c r="B526" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4878,7 +4878,7 @@
         <v>43224.6458333338</v>
       </c>
       <c r="B527" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4887,7 +4887,7 @@
         <v>43224.6527777782</v>
       </c>
       <c r="B528" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,7 +4896,7 @@
         <v>43224.6597222227</v>
       </c>
       <c r="B529" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,7 +4905,7 @@
         <v>43224.6666666671</v>
       </c>
       <c r="B530" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4914,7 +4914,7 @@
         <v>43224.6736111115</v>
       </c>
       <c r="B531" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4923,7 +4923,7 @@
         <v>43224.680555556</v>
       </c>
       <c r="B532" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4932,7 +4932,7 @@
         <v>43224.6875000004</v>
       </c>
       <c r="B533" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,7 +4941,7 @@
         <v>43224.6944444449</v>
       </c>
       <c r="B534" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4950,7 +4950,7 @@
         <v>43224.7013888893</v>
       </c>
       <c r="B535" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,7 +4959,7 @@
         <v>43224.7083333338</v>
       </c>
       <c r="B536" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4968,7 +4968,7 @@
         <v>43224.7152777782</v>
       </c>
       <c r="B537" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4977,7 +4977,7 @@
         <v>43224.7222222227</v>
       </c>
       <c r="B538" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,7 +4986,7 @@
         <v>43224.7291666671</v>
       </c>
       <c r="B539" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4995,7 @@
         <v>43224.7361111116</v>
       </c>
       <c r="B540" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5004,7 +5004,7 @@
         <v>43224.743055556</v>
       </c>
       <c r="B541" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5013,7 +5013,7 @@
         <v>43224.7500000004</v>
       </c>
       <c r="B542" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5022,7 +5022,7 @@
         <v>43224.7569444449</v>
       </c>
       <c r="B543" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,7 +5031,7 @@
         <v>43224.7638888893</v>
       </c>
       <c r="B544" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5040,7 +5040,7 @@
         <v>43224.7708333338</v>
       </c>
       <c r="B545" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,7 +5049,7 @@
         <v>43224.7777777782</v>
       </c>
       <c r="B546" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,7 +5058,7 @@
         <v>43224.7847222227</v>
       </c>
       <c r="B547" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5067,7 +5067,7 @@
         <v>43224.7916666671</v>
       </c>
       <c r="B548" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5076,7 +5076,7 @@
         <v>43224.7986111116</v>
       </c>
       <c r="B549" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,7 +5085,7 @@
         <v>43224.805555556</v>
       </c>
       <c r="B550" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>43224.8125000004</v>
       </c>
       <c r="B551" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,7 +5103,7 @@
         <v>43224.8194444449</v>
       </c>
       <c r="B552" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5112,7 +5112,7 @@
         <v>43224.8263888893</v>
       </c>
       <c r="B553" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5121,7 +5121,7 @@
         <v>43224.8333333338</v>
       </c>
       <c r="B554" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +5130,7 @@
         <v>43224.8402777782</v>
       </c>
       <c r="B555" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,7 +5139,7 @@
         <v>43224.8472222227</v>
       </c>
       <c r="B556" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5148,7 +5148,7 @@
         <v>43224.8541666671</v>
       </c>
       <c r="B557" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,7 +5157,7 @@
         <v>43224.8611111116</v>
       </c>
       <c r="B558" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5166,7 +5166,7 @@
         <v>43224.868055556</v>
       </c>
       <c r="B559" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5175,7 +5175,7 @@
         <v>43224.8750000004</v>
       </c>
       <c r="B560" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5184,7 +5184,7 @@
         <v>43224.8819444449</v>
       </c>
       <c r="B561" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5193,7 +5193,7 @@
         <v>43224.8888888893</v>
       </c>
       <c r="B562" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,7 +5202,7 @@
         <v>43224.8958333338</v>
       </c>
       <c r="B563" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,7 +5211,7 @@
         <v>43224.9027777782</v>
       </c>
       <c r="B564" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5220,7 +5220,7 @@
         <v>43224.9097222227</v>
       </c>
       <c r="B565" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5661,7 +5661,7 @@
         <v>43225.2500000005</v>
       </c>
       <c r="B614" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5670,7 +5670,7 @@
         <v>43225.2569444449</v>
       </c>
       <c r="B615" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5679,7 +5679,7 @@
         <v>43225.2638888894</v>
       </c>
       <c r="B616" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5688,7 +5688,7 @@
         <v>43225.2708333338</v>
       </c>
       <c r="B617" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5697,7 +5697,7 @@
         <v>43225.2777777783</v>
       </c>
       <c r="B618" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5706,7 +5706,7 @@
         <v>43225.2847222227</v>
       </c>
       <c r="B619" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5715,7 +5715,7 @@
         <v>43225.2916666672</v>
       </c>
       <c r="B620" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5724,7 +5724,7 @@
         <v>43225.2986111116</v>
       </c>
       <c r="B621" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5733,7 +5733,7 @@
         <v>43225.3055555561</v>
       </c>
       <c r="B622" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,7 +5742,7 @@
         <v>43225.3125000005</v>
       </c>
       <c r="B623" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5751,7 +5751,7 @@
         <v>43225.319444445</v>
       </c>
       <c r="B624" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5760,7 +5760,7 @@
         <v>43225.3263888894</v>
       </c>
       <c r="B625" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5769,7 +5769,7 @@
         <v>43225.3333333338</v>
       </c>
       <c r="B626" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5778,7 +5778,7 @@
         <v>43225.3402777783</v>
       </c>
       <c r="B627" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5787,7 +5787,7 @@
         <v>43225.3472222227</v>
       </c>
       <c r="B628" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5796,7 +5796,7 @@
         <v>43225.3541666672</v>
       </c>
       <c r="B629" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,7 +5805,7 @@
         <v>43225.3611111116</v>
       </c>
       <c r="B630" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,7 +5814,7 @@
         <v>43225.3680555561</v>
       </c>
       <c r="B631" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5823,7 +5823,7 @@
         <v>43225.3750000005</v>
       </c>
       <c r="B632" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5832,7 +5832,7 @@
         <v>43225.381944445</v>
       </c>
       <c r="B633" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5841,7 +5841,7 @@
         <v>43225.3888888894</v>
       </c>
       <c r="B634" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5850,7 +5850,7 @@
         <v>43225.3958333338</v>
       </c>
       <c r="B635" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,7 +5859,7 @@
         <v>43225.4027777783</v>
       </c>
       <c r="B636" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5868,7 +5868,7 @@
         <v>43225.4097222227</v>
       </c>
       <c r="B637" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5877,7 @@
         <v>43225.4166666672</v>
       </c>
       <c r="B638" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5886,7 +5886,7 @@
         <v>43225.4236111116</v>
       </c>
       <c r="B639" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="640" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5895,7 +5895,7 @@
         <v>43225.4305555561</v>
       </c>
       <c r="B640" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5904,7 +5904,7 @@
         <v>43225.4375000005</v>
       </c>
       <c r="B641" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5913,7 +5913,7 @@
         <v>43225.444444445</v>
       </c>
       <c r="B642" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5922,7 +5922,7 @@
         <v>43225.4513888894</v>
       </c>
       <c r="B643" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,7 +5931,7 @@
         <v>43225.4583333339</v>
       </c>
       <c r="B644" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5940,7 +5940,7 @@
         <v>43225.4652777783</v>
       </c>
       <c r="B645" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5949,7 +5949,7 @@
         <v>43225.4722222227</v>
       </c>
       <c r="B646" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5958,7 +5958,7 @@
         <v>43225.4791666672</v>
       </c>
       <c r="B647" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5967,7 +5967,7 @@
         <v>43225.4861111116</v>
       </c>
       <c r="B648" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5976,7 +5976,7 @@
         <v>43225.4930555561</v>
       </c>
       <c r="B649" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5985,7 +5985,7 @@
         <v>43225.5000000005</v>
       </c>
       <c r="B650" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5994,7 +5994,7 @@
         <v>43225.506944445</v>
       </c>
       <c r="B651" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6003,7 +6003,7 @@
         <v>43225.5138888894</v>
       </c>
       <c r="B652" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +6012,7 @@
         <v>43225.5208333339</v>
       </c>
       <c r="B653" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6021,7 +6021,7 @@
         <v>43225.5277777783</v>
       </c>
       <c r="B654" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6030,7 +6030,7 @@
         <v>43225.5347222228</v>
       </c>
       <c r="B655" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>43225.5416666672</v>
       </c>
       <c r="B656" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6048,7 +6048,7 @@
         <v>43225.5486111116</v>
       </c>
       <c r="B657" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6057,7 +6057,7 @@
         <v>43225.5555555561</v>
       </c>
       <c r="B658" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6066,7 +6066,7 @@
         <v>43225.5625000005</v>
       </c>
       <c r="B659" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6075,7 +6075,7 @@
         <v>43225.569444445</v>
       </c>
       <c r="B660" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6084,7 +6084,7 @@
         <v>43225.5763888894</v>
       </c>
       <c r="B661" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6093,7 +6093,7 @@
         <v>43225.5833333339</v>
       </c>
       <c r="B662" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6102,7 +6102,7 @@
         <v>43225.5902777783</v>
       </c>
       <c r="B663" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6111,7 +6111,7 @@
         <v>43225.5972222228</v>
       </c>
       <c r="B664" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6120,7 +6120,7 @@
         <v>43225.6041666672</v>
       </c>
       <c r="B665" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6129,7 +6129,7 @@
         <v>43225.6111111117</v>
       </c>
       <c r="B666" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6138,7 +6138,7 @@
         <v>43225.6180555561</v>
       </c>
       <c r="B667" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,7 +6147,7 @@
         <v>43225.6250000005</v>
       </c>
       <c r="B668" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6156,7 +6156,7 @@
         <v>43225.631944445</v>
       </c>
       <c r="B669" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6165,7 +6165,7 @@
         <v>43225.6388888894</v>
       </c>
       <c r="B670" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,7 +6174,7 @@
         <v>43225.6458333339</v>
       </c>
       <c r="B671" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6183,7 +6183,7 @@
         <v>43225.6527777783</v>
       </c>
       <c r="B672" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6192,7 +6192,7 @@
         <v>43225.6597222228</v>
       </c>
       <c r="B673" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6201,7 +6201,7 @@
         <v>43225.6666666672</v>
       </c>
       <c r="B674" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6210,7 +6210,7 @@
         <v>43225.6736111117</v>
       </c>
       <c r="B675" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6219,7 +6219,7 @@
         <v>43225.6805555561</v>
       </c>
       <c r="B676" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6228,7 +6228,7 @@
         <v>43225.6875000005</v>
       </c>
       <c r="B677" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6237,7 @@
         <v>43225.694444445</v>
       </c>
       <c r="B678" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,7 +6246,7 @@
         <v>43225.7013888894</v>
       </c>
       <c r="B679" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6255,7 +6255,7 @@
         <v>43225.7083333339</v>
       </c>
       <c r="B680" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,7 +6264,7 @@
         <v>43225.7152777783</v>
       </c>
       <c r="B681" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6273,7 +6273,7 @@
         <v>43225.7222222228</v>
       </c>
       <c r="B682" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6282,7 +6282,7 @@
         <v>43225.7291666672</v>
       </c>
       <c r="B683" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6291,7 +6291,7 @@
         <v>43225.7361111117</v>
       </c>
       <c r="B684" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,7 +6300,7 @@
         <v>43225.7430555561</v>
       </c>
       <c r="B685" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6309,7 +6309,7 @@
         <v>43225.7500000006</v>
       </c>
       <c r="B686" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6318,7 +6318,7 @@
         <v>43225.756944445</v>
       </c>
       <c r="B687" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6327,7 +6327,7 @@
         <v>43225.7638888894</v>
       </c>
       <c r="B688" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,7 +6336,7 @@
         <v>43225.7708333339</v>
       </c>
       <c r="B689" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6345,7 +6345,7 @@
         <v>43225.7777777783</v>
       </c>
       <c r="B690" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,7 +6354,7 @@
         <v>43225.7847222228</v>
       </c>
       <c r="B691" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6363,7 +6363,7 @@
         <v>43225.7916666672</v>
       </c>
       <c r="B692" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6372,7 +6372,7 @@
         <v>43225.7986111117</v>
       </c>
       <c r="B693" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6381,7 +6381,7 @@
         <v>43225.8055555561</v>
       </c>
       <c r="B694" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,7 +6390,7 @@
         <v>43225.8125000006</v>
       </c>
       <c r="B695" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="696" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6399,7 +6399,7 @@
         <v>43225.819444445</v>
       </c>
       <c r="B696" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6408,7 +6408,7 @@
         <v>43225.8263888895</v>
       </c>
       <c r="B697" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6417,7 +6417,7 @@
         <v>43225.8333333339</v>
       </c>
       <c r="B698" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="699" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6426,7 +6426,7 @@
         <v>43225.8402777783</v>
       </c>
       <c r="B699" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,7 +6435,7 @@
         <v>43225.8472222228</v>
       </c>
       <c r="B700" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6444,7 +6444,7 @@
         <v>43225.8541666672</v>
       </c>
       <c r="B701" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6453,7 +6453,7 @@
         <v>43225.8611111117</v>
       </c>
       <c r="B702" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6462,7 +6462,7 @@
         <v>43225.8680555561</v>
       </c>
       <c r="B703" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="704" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6471,7 @@
         <v>43225.8750000006</v>
       </c>
       <c r="B704" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6480,7 +6480,7 @@
         <v>43225.881944445</v>
       </c>
       <c r="B705" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,7 +6489,7 @@
         <v>43225.8888888895</v>
       </c>
       <c r="B706" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6498,7 +6498,7 @@
         <v>43225.8958333339</v>
       </c>
       <c r="B707" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6507,7 +6507,7 @@
         <v>43225.9027777783</v>
       </c>
       <c r="B708" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
original power buy price to 20 cents
</commit_message>
<xml_diff>
--- a/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
+++ b/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
@@ -130,8 +130,8 @@
   </sheetPr>
   <dimension ref="A1:B722"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A327" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C348" activeCellId="0" sqref="C348"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A698" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D710" activeCellId="0" sqref="D710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1773,7 +1773,7 @@
         <v>43222.2500000001</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,7 +1782,7 @@
         <v>43222.2569444446</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1791,7 @@
         <v>43222.263888889</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,7 +1800,7 @@
         <v>43222.2708333335</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,7 +1809,7 @@
         <v>43222.2777777779</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1818,7 @@
         <v>43222.2847222224</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1827,7 @@
         <v>43222.2916666668</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>43222.2986111113</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1845,7 @@
         <v>43222.3055555557</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
         <v>43222.3125000002</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1863,7 @@
         <v>43222.3194444446</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>43222.326388889</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1881,7 @@
         <v>43222.3333333335</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1890,7 @@
         <v>43222.3402777779</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,7 +1899,7 @@
         <v>43222.3472222224</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1908,7 @@
         <v>43222.3541666668</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +1917,7 @@
         <v>43222.3611111113</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1926,7 @@
         <v>43222.3680555557</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
         <v>43222.3750000002</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1944,7 @@
         <v>43222.3819444446</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,7 +1953,7 @@
         <v>43222.3888888891</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,7 +1962,7 @@
         <v>43222.3958333335</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>43222.4027777779</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1980,7 @@
         <v>43222.4097222224</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1989,7 @@
         <v>43222.4166666668</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +1998,7 @@
         <v>43222.4236111113</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,7 +2007,7 @@
         <v>43222.4305555557</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2016,7 @@
         <v>43222.4375000002</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2025,7 @@
         <v>43222.4444444446</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2034,7 @@
         <v>43222.4513888891</v>
       </c>
       <c r="B211" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2043,7 @@
         <v>43222.4583333335</v>
       </c>
       <c r="B212" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,7 +2052,7 @@
         <v>43222.4652777779</v>
       </c>
       <c r="B213" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2061,7 @@
         <v>43222.4722222224</v>
       </c>
       <c r="B214" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>43222.4791666668</v>
       </c>
       <c r="B215" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2079,7 @@
         <v>43222.4861111113</v>
       </c>
       <c r="B216" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2088,7 @@
         <v>43222.4930555557</v>
       </c>
       <c r="B217" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,7 +2097,7 @@
         <v>43222.5000000002</v>
       </c>
       <c r="B218" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2106,7 @@
         <v>43222.5069444446</v>
       </c>
       <c r="B219" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +2115,7 @@
         <v>43222.5138888891</v>
       </c>
       <c r="B220" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2124,7 @@
         <v>43222.5208333335</v>
       </c>
       <c r="B221" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2133,7 @@
         <v>43222.527777778</v>
       </c>
       <c r="B222" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2142,7 @@
         <v>43222.5347222224</v>
       </c>
       <c r="B223" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,7 +2151,7 @@
         <v>43222.5416666669</v>
       </c>
       <c r="B224" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>43222.5486111113</v>
       </c>
       <c r="B225" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2169,7 @@
         <v>43222.5555555557</v>
       </c>
       <c r="B226" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2178,7 @@
         <v>43222.5625000002</v>
       </c>
       <c r="B227" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2187,7 @@
         <v>43222.5694444446</v>
       </c>
       <c r="B228" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2196,7 @@
         <v>43222.5763888891</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2205,7 @@
         <v>43222.5833333335</v>
       </c>
       <c r="B230" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,7 +2214,7 @@
         <v>43222.590277778</v>
       </c>
       <c r="B231" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2223,7 @@
         <v>43222.5972222224</v>
       </c>
       <c r="B232" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2232,7 @@
         <v>43222.6041666669</v>
       </c>
       <c r="B233" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,7 +2241,7 @@
         <v>43222.6111111113</v>
       </c>
       <c r="B234" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2250,7 @@
         <v>43222.6180555557</v>
       </c>
       <c r="B235" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,7 +2259,7 @@
         <v>43222.6250000002</v>
       </c>
       <c r="B236" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2268,7 @@
         <v>43222.6319444446</v>
       </c>
       <c r="B237" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2277,7 @@
         <v>43222.6388888891</v>
       </c>
       <c r="B238" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>43222.6458333335</v>
       </c>
       <c r="B239" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,7 +2295,7 @@
         <v>43222.652777778</v>
       </c>
       <c r="B240" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,7 +2304,7 @@
         <v>43222.6597222224</v>
       </c>
       <c r="B241" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2313,7 @@
         <v>43222.6666666669</v>
       </c>
       <c r="B242" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2322,7 @@
         <v>43222.6736111113</v>
       </c>
       <c r="B243" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,7 +2331,7 @@
         <v>43222.6805555558</v>
       </c>
       <c r="B244" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2340,7 @@
         <v>43222.6875000002</v>
       </c>
       <c r="B245" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2349,7 @@
         <v>43222.6944444446</v>
       </c>
       <c r="B246" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,7 +2358,7 @@
         <v>43222.7013888891</v>
       </c>
       <c r="B247" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,7 +2367,7 @@
         <v>43222.7083333335</v>
       </c>
       <c r="B248" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,7 +2376,7 @@
         <v>43222.715277778</v>
       </c>
       <c r="B249" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>43222.7222222224</v>
       </c>
       <c r="B250" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2394,7 @@
         <v>43222.7291666669</v>
       </c>
       <c r="B251" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2403,7 @@
         <v>43222.7361111113</v>
       </c>
       <c r="B252" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,7 +2412,7 @@
         <v>43222.7430555558</v>
       </c>
       <c r="B253" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2421,7 @@
         <v>43222.7500000002</v>
       </c>
       <c r="B254" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2430,7 @@
         <v>43222.7569444447</v>
       </c>
       <c r="B255" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,7 +2439,7 @@
         <v>43222.7638888891</v>
       </c>
       <c r="B256" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,7 +2448,7 @@
         <v>43222.7708333335</v>
       </c>
       <c r="B257" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2457,7 @@
         <v>43222.777777778</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2466,7 @@
         <v>43222.7847222224</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2475,7 @@
         <v>43222.7916666669</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>43222.7986111113</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2493,7 @@
         <v>43222.8055555558</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2502,7 @@
         <v>43222.8125000002</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,7 +2511,7 @@
         <v>43222.8194444447</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2520,7 @@
         <v>43222.8263888891</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,7 +2529,7 @@
         <v>43222.8333333335</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,7 +2538,7 @@
         <v>43222.840277778</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2547,7 @@
         <v>43222.8472222224</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,7 +2556,7 @@
         <v>43222.8541666669</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2565,7 @@
         <v>43222.8611111113</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,7 +2574,7 @@
         <v>43222.8680555558</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>43222.8750000002</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2592,7 @@
         <v>43222.8819444447</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,7 +2601,7 @@
         <v>43222.8888888891</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2610,7 @@
         <v>43222.8958333336</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2619,7 @@
         <v>43222.902777778</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,7 +2628,7 @@
         <v>43222.9097222225</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,7 +3069,7 @@
         <v>43223.2500000003</v>
       </c>
       <c r="B326" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,7 +3078,7 @@
         <v>43223.2569444447</v>
       </c>
       <c r="B327" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,7 +3087,7 @@
         <v>43223.2638888892</v>
       </c>
       <c r="B328" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,7 +3096,7 @@
         <v>43223.2708333336</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,7 +3105,7 @@
         <v>43223.277777778</v>
       </c>
       <c r="B330" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,7 +3114,7 @@
         <v>43223.2847222225</v>
       </c>
       <c r="B331" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,7 +3123,7 @@
         <v>43223.2916666669</v>
       </c>
       <c r="B332" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3132,7 @@
         <v>43223.2986111114</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,7 +3141,7 @@
         <v>43223.3055555558</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,7 +3150,7 @@
         <v>43223.3125000003</v>
       </c>
       <c r="B335" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,7 +3159,7 @@
         <v>43223.3194444447</v>
       </c>
       <c r="B336" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3168,7 @@
         <v>43223.3263888892</v>
       </c>
       <c r="B337" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,7 +3177,7 @@
         <v>43223.3333333336</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3186,7 @@
         <v>43223.340277778</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,7 +3195,7 @@
         <v>43223.3472222225</v>
       </c>
       <c r="B340" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,7 +3204,7 @@
         <v>43223.3541666669</v>
       </c>
       <c r="B341" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,7 +3213,7 @@
         <v>43223.3611111114</v>
       </c>
       <c r="B342" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3222,7 +3222,7 @@
         <v>43223.3680555558</v>
       </c>
       <c r="B343" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,7 +3231,7 @@
         <v>43223.3750000003</v>
       </c>
       <c r="B344" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,7 +3240,7 @@
         <v>43223.3819444447</v>
       </c>
       <c r="B345" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,7 +3249,7 @@
         <v>43223.3888888892</v>
       </c>
       <c r="B346" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,7 +3258,7 @@
         <v>43223.3958333336</v>
       </c>
       <c r="B347" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,7 +3267,7 @@
         <v>43223.4027777781</v>
       </c>
       <c r="B348" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,7 +3276,7 @@
         <v>43223.4097222225</v>
       </c>
       <c r="B349" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3285,7 @@
         <v>43223.416666667</v>
       </c>
       <c r="B350" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3294,7 +3294,7 @@
         <v>43223.4236111114</v>
       </c>
       <c r="B351" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,7 +3303,7 @@
         <v>43223.4305555558</v>
       </c>
       <c r="B352" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,7 +3312,7 @@
         <v>43223.4375000003</v>
       </c>
       <c r="B353" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,7 +3321,7 @@
         <v>43223.4444444447</v>
       </c>
       <c r="B354" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,7 +3330,7 @@
         <v>43223.4513888892</v>
       </c>
       <c r="B355" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3339,7 @@
         <v>43223.4583333336</v>
       </c>
       <c r="B356" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3348,7 +3348,7 @@
         <v>43223.4652777781</v>
       </c>
       <c r="B357" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3357,7 @@
         <v>43223.4722222225</v>
       </c>
       <c r="B358" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,7 +3366,7 @@
         <v>43223.479166667</v>
       </c>
       <c r="B359" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,7 +3375,7 @@
         <v>43223.4861111114</v>
       </c>
       <c r="B360" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3384,7 @@
         <v>43223.4930555558</v>
       </c>
       <c r="B361" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,7 +3393,7 @@
         <v>43223.5000000003</v>
       </c>
       <c r="B362" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,7 +3402,7 @@
         <v>43223.5069444447</v>
       </c>
       <c r="B363" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,7 +3411,7 @@
         <v>43223.5138888892</v>
       </c>
       <c r="B364" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,7 +3420,7 @@
         <v>43223.5208333336</v>
       </c>
       <c r="B365" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,7 +3429,7 @@
         <v>43223.5277777781</v>
       </c>
       <c r="B366" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3438,7 +3438,7 @@
         <v>43223.5347222225</v>
       </c>
       <c r="B367" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3447,7 @@
         <v>43223.541666667</v>
       </c>
       <c r="B368" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3456,7 @@
         <v>43223.5486111114</v>
       </c>
       <c r="B369" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,7 +3465,7 @@
         <v>43223.5555555559</v>
       </c>
       <c r="B370" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,7 +3474,7 @@
         <v>43223.5625000003</v>
       </c>
       <c r="B371" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3483,7 @@
         <v>43223.5694444448</v>
       </c>
       <c r="B372" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3492,7 +3492,7 @@
         <v>43223.5763888892</v>
       </c>
       <c r="B373" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,7 +3501,7 @@
         <v>43223.5833333336</v>
       </c>
       <c r="B374" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3510,7 +3510,7 @@
         <v>43223.5902777781</v>
       </c>
       <c r="B375" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,7 +3519,7 @@
         <v>43223.5972222225</v>
       </c>
       <c r="B376" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3528,7 +3528,7 @@
         <v>43223.604166667</v>
       </c>
       <c r="B377" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,7 +3537,7 @@
         <v>43223.6111111114</v>
       </c>
       <c r="B378" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3546,7 @@
         <v>43223.6180555559</v>
       </c>
       <c r="B379" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,7 +3555,7 @@
         <v>43223.6250000003</v>
       </c>
       <c r="B380" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +3564,7 @@
         <v>43223.6319444448</v>
       </c>
       <c r="B381" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,7 +3573,7 @@
         <v>43223.6388888892</v>
       </c>
       <c r="B382" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3582,7 @@
         <v>43223.6458333336</v>
       </c>
       <c r="B383" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,7 +3591,7 @@
         <v>43223.6527777781</v>
       </c>
       <c r="B384" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,7 +3600,7 @@
         <v>43223.6597222225</v>
       </c>
       <c r="B385" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,7 +3609,7 @@
         <v>43223.666666667</v>
       </c>
       <c r="B386" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3618,7 @@
         <v>43223.6736111114</v>
       </c>
       <c r="B387" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,7 +3627,7 @@
         <v>43223.6805555559</v>
       </c>
       <c r="B388" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,7 +3636,7 @@
         <v>43223.6875000003</v>
       </c>
       <c r="B389" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,7 +3645,7 @@
         <v>43223.6944444448</v>
       </c>
       <c r="B390" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3654,7 +3654,7 @@
         <v>43223.7013888892</v>
       </c>
       <c r="B391" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3663,7 @@
         <v>43223.7083333337</v>
       </c>
       <c r="B392" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,7 +3672,7 @@
         <v>43223.7152777781</v>
       </c>
       <c r="B393" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,7 +3681,7 @@
         <v>43223.7222222225</v>
       </c>
       <c r="B394" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3690,7 +3690,7 @@
         <v>43223.729166667</v>
       </c>
       <c r="B395" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,7 +3699,7 @@
         <v>43223.7361111114</v>
       </c>
       <c r="B396" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,7 +3708,7 @@
         <v>43223.7430555559</v>
       </c>
       <c r="B397" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,7 +3717,7 @@
         <v>43223.7500000003</v>
       </c>
       <c r="B398" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3726,7 @@
         <v>43223.7569444448</v>
       </c>
       <c r="B399" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,7 +3735,7 @@
         <v>43223.7638888892</v>
       </c>
       <c r="B400" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,7 +3744,7 @@
         <v>43223.7708333337</v>
       </c>
       <c r="B401" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,7 +3753,7 @@
         <v>43223.7777777781</v>
       </c>
       <c r="B402" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3762,7 @@
         <v>43223.7847222226</v>
       </c>
       <c r="B403" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,7 +3771,7 @@
         <v>43223.791666667</v>
       </c>
       <c r="B404" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3780,7 +3780,7 @@
         <v>43223.7986111114</v>
       </c>
       <c r="B405" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,7 +3789,7 @@
         <v>43223.8055555559</v>
       </c>
       <c r="B406" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,7 +3798,7 @@
         <v>43223.8125000003</v>
       </c>
       <c r="B407" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,7 +3807,7 @@
         <v>43223.8194444448</v>
       </c>
       <c r="B408" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,7 +3816,7 @@
         <v>43223.8263888892</v>
       </c>
       <c r="B409" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,7 +3825,7 @@
         <v>43223.8333333337</v>
       </c>
       <c r="B410" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,7 +3834,7 @@
         <v>43223.8402777781</v>
       </c>
       <c r="B411" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3843,7 @@
         <v>43223.8472222226</v>
       </c>
       <c r="B412" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,7 +3852,7 @@
         <v>43223.854166667</v>
       </c>
       <c r="B413" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>43223.8611111114</v>
       </c>
       <c r="B414" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3870,7 +3870,7 @@
         <v>43223.8680555559</v>
       </c>
       <c r="B415" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,7 +3879,7 @@
         <v>43223.8750000003</v>
       </c>
       <c r="B416" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3888,7 +3888,7 @@
         <v>43223.8819444448</v>
       </c>
       <c r="B417" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,7 +3897,7 @@
         <v>43223.8888888892</v>
       </c>
       <c r="B418" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,7 +3906,7 @@
         <v>43223.8958333337</v>
       </c>
       <c r="B419" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3915,7 @@
         <v>43223.9027777781</v>
       </c>
       <c r="B420" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,7 +3924,7 @@
         <v>43223.9097222226</v>
       </c>
       <c r="B421" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4365,7 +4365,7 @@
         <v>43224.2500000004</v>
       </c>
       <c r="B470" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4374,7 @@
         <v>43224.2569444448</v>
       </c>
       <c r="B471" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4383,7 +4383,7 @@
         <v>43224.2638888893</v>
       </c>
       <c r="B472" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,7 +4392,7 @@
         <v>43224.2708333337</v>
       </c>
       <c r="B473" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4401,7 +4401,7 @@
         <v>43224.2777777782</v>
       </c>
       <c r="B474" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4410,7 @@
         <v>43224.2847222226</v>
       </c>
       <c r="B475" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,7 +4419,7 @@
         <v>43224.2916666671</v>
       </c>
       <c r="B476" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,7 +4428,7 @@
         <v>43224.2986111115</v>
       </c>
       <c r="B477" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,7 +4437,7 @@
         <v>43224.3055555559</v>
       </c>
       <c r="B478" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,7 +4446,7 @@
         <v>43224.3125000004</v>
       </c>
       <c r="B479" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4455,7 +4455,7 @@
         <v>43224.3194444448</v>
       </c>
       <c r="B480" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4464,7 @@
         <v>43224.3263888893</v>
       </c>
       <c r="B481" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,7 +4473,7 @@
         <v>43224.3333333337</v>
       </c>
       <c r="B482" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,7 +4482,7 @@
         <v>43224.3402777782</v>
       </c>
       <c r="B483" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4491,7 +4491,7 @@
         <v>43224.3472222226</v>
       </c>
       <c r="B484" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,7 +4500,7 @@
         <v>43224.3541666671</v>
       </c>
       <c r="B485" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4509,7 +4509,7 @@
         <v>43224.3611111115</v>
       </c>
       <c r="B486" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4518,7 @@
         <v>43224.3680555559</v>
       </c>
       <c r="B487" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,7 +4527,7 @@
         <v>43224.3750000004</v>
       </c>
       <c r="B488" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,7 @@
         <v>43224.3819444448</v>
       </c>
       <c r="B489" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4545,7 +4545,7 @@
         <v>43224.3888888893</v>
       </c>
       <c r="B490" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,7 +4554,7 @@
         <v>43224.3958333337</v>
       </c>
       <c r="B491" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4563,7 +4563,7 @@
         <v>43224.4027777782</v>
       </c>
       <c r="B492" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4572,7 +4572,7 @@
         <v>43224.4097222226</v>
       </c>
       <c r="B493" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4581,7 +4581,7 @@
         <v>43224.4166666671</v>
       </c>
       <c r="B494" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,7 +4590,7 @@
         <v>43224.4236111115</v>
       </c>
       <c r="B495" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,7 +4599,7 @@
         <v>43224.430555556</v>
       </c>
       <c r="B496" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,7 +4608,7 @@
         <v>43224.4375000004</v>
       </c>
       <c r="B497" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,7 +4617,7 @@
         <v>43224.4444444449</v>
       </c>
       <c r="B498" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4626,7 +4626,7 @@
         <v>43224.4513888893</v>
       </c>
       <c r="B499" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4635,7 +4635,7 @@
         <v>43224.4583333337</v>
       </c>
       <c r="B500" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4644,7 +4644,7 @@
         <v>43224.4652777782</v>
       </c>
       <c r="B501" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4653,7 +4653,7 @@
         <v>43224.4722222226</v>
       </c>
       <c r="B502" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4662,7 +4662,7 @@
         <v>43224.4791666671</v>
       </c>
       <c r="B503" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4671,7 +4671,7 @@
         <v>43224.4861111115</v>
       </c>
       <c r="B504" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4680,7 @@
         <v>43224.493055556</v>
       </c>
       <c r="B505" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4689,7 +4689,7 @@
         <v>43224.5000000004</v>
       </c>
       <c r="B506" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4698,7 +4698,7 @@
         <v>43224.5069444449</v>
       </c>
       <c r="B507" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,7 +4707,7 @@
         <v>43224.5138888893</v>
       </c>
       <c r="B508" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4716,7 +4716,7 @@
         <v>43224.5208333337</v>
       </c>
       <c r="B509" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,7 +4725,7 @@
         <v>43224.5277777782</v>
       </c>
       <c r="B510" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,7 +4734,7 @@
         <v>43224.5347222226</v>
       </c>
       <c r="B511" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4743,7 +4743,7 @@
         <v>43224.5416666671</v>
       </c>
       <c r="B512" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4752,7 +4752,7 @@
         <v>43224.5486111115</v>
       </c>
       <c r="B513" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4761,7 +4761,7 @@
         <v>43224.555555556</v>
       </c>
       <c r="B514" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,7 +4770,7 @@
         <v>43224.5625000004</v>
       </c>
       <c r="B515" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4779,7 +4779,7 @@
         <v>43224.5694444449</v>
       </c>
       <c r="B516" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4788,7 +4788,7 @@
         <v>43224.5763888893</v>
       </c>
       <c r="B517" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4797,7 @@
         <v>43224.5833333338</v>
       </c>
       <c r="B518" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4806,7 +4806,7 @@
         <v>43224.5902777782</v>
       </c>
       <c r="B519" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4815,7 +4815,7 @@
         <v>43224.5972222226</v>
       </c>
       <c r="B520" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4824,7 +4824,7 @@
         <v>43224.6041666671</v>
       </c>
       <c r="B521" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4833,7 @@
         <v>43224.6111111115</v>
       </c>
       <c r="B522" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,7 +4842,7 @@
         <v>43224.618055556</v>
       </c>
       <c r="B523" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,7 +4851,7 @@
         <v>43224.6250000004</v>
       </c>
       <c r="B524" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4860,7 +4860,7 @@
         <v>43224.6319444449</v>
       </c>
       <c r="B525" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4869,7 +4869,7 @@
         <v>43224.6388888893</v>
       </c>
       <c r="B526" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4878,7 +4878,7 @@
         <v>43224.6458333338</v>
       </c>
       <c r="B527" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4887,7 +4887,7 @@
         <v>43224.6527777782</v>
       </c>
       <c r="B528" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,7 +4896,7 @@
         <v>43224.6597222227</v>
       </c>
       <c r="B529" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,7 +4905,7 @@
         <v>43224.6666666671</v>
       </c>
       <c r="B530" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4914,7 +4914,7 @@
         <v>43224.6736111115</v>
       </c>
       <c r="B531" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4923,7 +4923,7 @@
         <v>43224.680555556</v>
       </c>
       <c r="B532" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4932,7 +4932,7 @@
         <v>43224.6875000004</v>
       </c>
       <c r="B533" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,7 +4941,7 @@
         <v>43224.6944444449</v>
       </c>
       <c r="B534" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4950,7 +4950,7 @@
         <v>43224.7013888893</v>
       </c>
       <c r="B535" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,7 +4959,7 @@
         <v>43224.7083333338</v>
       </c>
       <c r="B536" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4968,7 +4968,7 @@
         <v>43224.7152777782</v>
       </c>
       <c r="B537" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4977,7 +4977,7 @@
         <v>43224.7222222227</v>
       </c>
       <c r="B538" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,7 +4986,7 @@
         <v>43224.7291666671</v>
       </c>
       <c r="B539" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4995,7 @@
         <v>43224.7361111116</v>
       </c>
       <c r="B540" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5004,7 +5004,7 @@
         <v>43224.743055556</v>
       </c>
       <c r="B541" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5013,7 +5013,7 @@
         <v>43224.7500000004</v>
       </c>
       <c r="B542" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5022,7 +5022,7 @@
         <v>43224.7569444449</v>
       </c>
       <c r="B543" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,7 +5031,7 @@
         <v>43224.7638888893</v>
       </c>
       <c r="B544" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5040,7 +5040,7 @@
         <v>43224.7708333338</v>
       </c>
       <c r="B545" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,7 +5049,7 @@
         <v>43224.7777777782</v>
       </c>
       <c r="B546" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,7 +5058,7 @@
         <v>43224.7847222227</v>
       </c>
       <c r="B547" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5067,7 +5067,7 @@
         <v>43224.7916666671</v>
       </c>
       <c r="B548" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5076,7 +5076,7 @@
         <v>43224.7986111116</v>
       </c>
       <c r="B549" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,7 +5085,7 @@
         <v>43224.805555556</v>
       </c>
       <c r="B550" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>43224.8125000004</v>
       </c>
       <c r="B551" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,7 +5103,7 @@
         <v>43224.8194444449</v>
       </c>
       <c r="B552" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5112,7 +5112,7 @@
         <v>43224.8263888893</v>
       </c>
       <c r="B553" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5121,7 +5121,7 @@
         <v>43224.8333333338</v>
       </c>
       <c r="B554" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +5130,7 @@
         <v>43224.8402777782</v>
       </c>
       <c r="B555" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,7 +5139,7 @@
         <v>43224.8472222227</v>
       </c>
       <c r="B556" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5148,7 +5148,7 @@
         <v>43224.8541666671</v>
       </c>
       <c r="B557" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,7 +5157,7 @@
         <v>43224.8611111116</v>
       </c>
       <c r="B558" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5166,7 +5166,7 @@
         <v>43224.868055556</v>
       </c>
       <c r="B559" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5175,7 +5175,7 @@
         <v>43224.8750000004</v>
       </c>
       <c r="B560" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5184,7 +5184,7 @@
         <v>43224.8819444449</v>
       </c>
       <c r="B561" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5193,7 +5193,7 @@
         <v>43224.8888888893</v>
       </c>
       <c r="B562" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,7 +5202,7 @@
         <v>43224.8958333338</v>
       </c>
       <c r="B563" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,7 +5211,7 @@
         <v>43224.9027777782</v>
       </c>
       <c r="B564" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5220,7 +5220,7 @@
         <v>43224.9097222227</v>
       </c>
       <c r="B565" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5661,7 +5661,7 @@
         <v>43225.2500000005</v>
       </c>
       <c r="B614" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5670,7 +5670,7 @@
         <v>43225.2569444449</v>
       </c>
       <c r="B615" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5679,7 +5679,7 @@
         <v>43225.2638888894</v>
       </c>
       <c r="B616" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5688,7 +5688,7 @@
         <v>43225.2708333338</v>
       </c>
       <c r="B617" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5697,7 +5697,7 @@
         <v>43225.2777777783</v>
       </c>
       <c r="B618" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5706,7 +5706,7 @@
         <v>43225.2847222227</v>
       </c>
       <c r="B619" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5715,7 +5715,7 @@
         <v>43225.2916666672</v>
       </c>
       <c r="B620" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5724,7 +5724,7 @@
         <v>43225.2986111116</v>
       </c>
       <c r="B621" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5733,7 +5733,7 @@
         <v>43225.3055555561</v>
       </c>
       <c r="B622" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,7 +5742,7 @@
         <v>43225.3125000005</v>
       </c>
       <c r="B623" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5751,7 +5751,7 @@
         <v>43225.319444445</v>
       </c>
       <c r="B624" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5760,7 +5760,7 @@
         <v>43225.3263888894</v>
       </c>
       <c r="B625" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5769,7 +5769,7 @@
         <v>43225.3333333338</v>
       </c>
       <c r="B626" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5778,7 +5778,7 @@
         <v>43225.3402777783</v>
       </c>
       <c r="B627" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5787,7 +5787,7 @@
         <v>43225.3472222227</v>
       </c>
       <c r="B628" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5796,7 +5796,7 @@
         <v>43225.3541666672</v>
       </c>
       <c r="B629" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,7 +5805,7 @@
         <v>43225.3611111116</v>
       </c>
       <c r="B630" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,7 +5814,7 @@
         <v>43225.3680555561</v>
       </c>
       <c r="B631" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5823,7 +5823,7 @@
         <v>43225.3750000005</v>
       </c>
       <c r="B632" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5832,7 +5832,7 @@
         <v>43225.381944445</v>
       </c>
       <c r="B633" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5841,7 +5841,7 @@
         <v>43225.3888888894</v>
       </c>
       <c r="B634" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5850,7 +5850,7 @@
         <v>43225.3958333338</v>
       </c>
       <c r="B635" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,7 +5859,7 @@
         <v>43225.4027777783</v>
       </c>
       <c r="B636" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5868,7 +5868,7 @@
         <v>43225.4097222227</v>
       </c>
       <c r="B637" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5877,7 @@
         <v>43225.4166666672</v>
       </c>
       <c r="B638" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5886,7 +5886,7 @@
         <v>43225.4236111116</v>
       </c>
       <c r="B639" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="640" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5895,7 +5895,7 @@
         <v>43225.4305555561</v>
       </c>
       <c r="B640" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5904,7 +5904,7 @@
         <v>43225.4375000005</v>
       </c>
       <c r="B641" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5913,7 +5913,7 @@
         <v>43225.444444445</v>
       </c>
       <c r="B642" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5922,7 +5922,7 @@
         <v>43225.4513888894</v>
       </c>
       <c r="B643" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,7 +5931,7 @@
         <v>43225.4583333339</v>
       </c>
       <c r="B644" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5940,7 +5940,7 @@
         <v>43225.4652777783</v>
       </c>
       <c r="B645" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5949,7 +5949,7 @@
         <v>43225.4722222227</v>
       </c>
       <c r="B646" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5958,7 +5958,7 @@
         <v>43225.4791666672</v>
       </c>
       <c r="B647" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5967,7 +5967,7 @@
         <v>43225.4861111116</v>
       </c>
       <c r="B648" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5976,7 +5976,7 @@
         <v>43225.4930555561</v>
       </c>
       <c r="B649" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5985,7 +5985,7 @@
         <v>43225.5000000005</v>
       </c>
       <c r="B650" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5994,7 +5994,7 @@
         <v>43225.506944445</v>
       </c>
       <c r="B651" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6003,7 +6003,7 @@
         <v>43225.5138888894</v>
       </c>
       <c r="B652" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +6012,7 @@
         <v>43225.5208333339</v>
       </c>
       <c r="B653" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6021,7 +6021,7 @@
         <v>43225.5277777783</v>
       </c>
       <c r="B654" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6030,7 +6030,7 @@
         <v>43225.5347222228</v>
       </c>
       <c r="B655" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>43225.5416666672</v>
       </c>
       <c r="B656" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6048,7 +6048,7 @@
         <v>43225.5486111116</v>
       </c>
       <c r="B657" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6057,7 +6057,7 @@
         <v>43225.5555555561</v>
       </c>
       <c r="B658" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6066,7 +6066,7 @@
         <v>43225.5625000005</v>
       </c>
       <c r="B659" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6075,7 +6075,7 @@
         <v>43225.569444445</v>
       </c>
       <c r="B660" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6084,7 +6084,7 @@
         <v>43225.5763888894</v>
       </c>
       <c r="B661" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6093,7 +6093,7 @@
         <v>43225.5833333339</v>
       </c>
       <c r="B662" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6102,7 +6102,7 @@
         <v>43225.5902777783</v>
       </c>
       <c r="B663" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6111,7 +6111,7 @@
         <v>43225.5972222228</v>
       </c>
       <c r="B664" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6120,7 +6120,7 @@
         <v>43225.6041666672</v>
       </c>
       <c r="B665" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6129,7 +6129,7 @@
         <v>43225.6111111117</v>
       </c>
       <c r="B666" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6138,7 +6138,7 @@
         <v>43225.6180555561</v>
       </c>
       <c r="B667" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,7 +6147,7 @@
         <v>43225.6250000005</v>
       </c>
       <c r="B668" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6156,7 +6156,7 @@
         <v>43225.631944445</v>
       </c>
       <c r="B669" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6165,7 +6165,7 @@
         <v>43225.6388888894</v>
       </c>
       <c r="B670" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,7 +6174,7 @@
         <v>43225.6458333339</v>
       </c>
       <c r="B671" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6183,7 +6183,7 @@
         <v>43225.6527777783</v>
       </c>
       <c r="B672" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6192,7 +6192,7 @@
         <v>43225.6597222228</v>
       </c>
       <c r="B673" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6201,7 +6201,7 @@
         <v>43225.6666666672</v>
       </c>
       <c r="B674" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6210,7 +6210,7 @@
         <v>43225.6736111117</v>
       </c>
       <c r="B675" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6219,7 +6219,7 @@
         <v>43225.6805555561</v>
       </c>
       <c r="B676" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6228,7 +6228,7 @@
         <v>43225.6875000005</v>
       </c>
       <c r="B677" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6237,7 @@
         <v>43225.694444445</v>
       </c>
       <c r="B678" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,7 +6246,7 @@
         <v>43225.7013888894</v>
       </c>
       <c r="B679" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6255,7 +6255,7 @@
         <v>43225.7083333339</v>
       </c>
       <c r="B680" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,7 +6264,7 @@
         <v>43225.7152777783</v>
       </c>
       <c r="B681" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6273,7 +6273,7 @@
         <v>43225.7222222228</v>
       </c>
       <c r="B682" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6282,7 +6282,7 @@
         <v>43225.7291666672</v>
       </c>
       <c r="B683" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6291,7 +6291,7 @@
         <v>43225.7361111117</v>
       </c>
       <c r="B684" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,7 +6300,7 @@
         <v>43225.7430555561</v>
       </c>
       <c r="B685" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6309,7 +6309,7 @@
         <v>43225.7500000006</v>
       </c>
       <c r="B686" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6318,7 +6318,7 @@
         <v>43225.756944445</v>
       </c>
       <c r="B687" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6327,7 +6327,7 @@
         <v>43225.7638888894</v>
       </c>
       <c r="B688" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,7 +6336,7 @@
         <v>43225.7708333339</v>
       </c>
       <c r="B689" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6345,7 +6345,7 @@
         <v>43225.7777777783</v>
       </c>
       <c r="B690" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,7 +6354,7 @@
         <v>43225.7847222228</v>
       </c>
       <c r="B691" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6363,7 +6363,7 @@
         <v>43225.7916666672</v>
       </c>
       <c r="B692" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6372,7 +6372,7 @@
         <v>43225.7986111117</v>
       </c>
       <c r="B693" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6381,7 +6381,7 @@
         <v>43225.8055555561</v>
       </c>
       <c r="B694" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,7 +6390,7 @@
         <v>43225.8125000006</v>
       </c>
       <c r="B695" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="696" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6399,7 +6399,7 @@
         <v>43225.819444445</v>
       </c>
       <c r="B696" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6408,7 +6408,7 @@
         <v>43225.8263888895</v>
       </c>
       <c r="B697" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6417,7 +6417,7 @@
         <v>43225.8333333339</v>
       </c>
       <c r="B698" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="699" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6426,7 +6426,7 @@
         <v>43225.8402777783</v>
       </c>
       <c r="B699" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,7 +6435,7 @@
         <v>43225.8472222228</v>
       </c>
       <c r="B700" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6444,7 +6444,7 @@
         <v>43225.8541666672</v>
       </c>
       <c r="B701" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6453,7 +6453,7 @@
         <v>43225.8611111117</v>
       </c>
       <c r="B702" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6462,7 +6462,7 @@
         <v>43225.8680555561</v>
       </c>
       <c r="B703" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="704" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6471,7 @@
         <v>43225.8750000006</v>
       </c>
       <c r="B704" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6480,7 +6480,7 @@
         <v>43225.881944445</v>
       </c>
       <c r="B705" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,7 +6489,7 @@
         <v>43225.8888888895</v>
       </c>
       <c r="B706" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6498,7 +6498,7 @@
         <v>43225.8958333339</v>
       </c>
       <c r="B707" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6507,7 +6507,7 @@
         <v>43225.9027777783</v>
       </c>
       <c r="B708" s="0" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
mpc boilers linearized and working well
</commit_message>
<xml_diff>
--- a/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
+++ b/EMS_simulation/data_input/energy_buy_price_10min_granularity.xlsx
@@ -130,8 +130,8 @@
   </sheetPr>
   <dimension ref="A1:B722"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A698" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D710" activeCellId="0" sqref="D710"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A251" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D277" activeCellId="0" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1773,7 +1773,7 @@
         <v>43222.2500000001</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,7 +1782,7 @@
         <v>43222.2569444446</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1791,7 @@
         <v>43222.263888889</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,7 +1800,7 @@
         <v>43222.2708333335</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,7 +1809,7 @@
         <v>43222.2777777779</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1818,7 @@
         <v>43222.2847222224</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1827,7 @@
         <v>43222.2916666668</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>43222.2986111113</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1845,7 @@
         <v>43222.3055555557</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
         <v>43222.3125000002</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1863,7 @@
         <v>43222.3194444446</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>43222.326388889</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1881,7 @@
         <v>43222.3333333335</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1890,7 @@
         <v>43222.3402777779</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,7 +1899,7 @@
         <v>43222.3472222224</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1908,7 @@
         <v>43222.3541666668</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +1917,7 @@
         <v>43222.3611111113</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1926,7 @@
         <v>43222.3680555557</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
         <v>43222.3750000002</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1944,7 @@
         <v>43222.3819444446</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,7 +1953,7 @@
         <v>43222.3888888891</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,7 +1962,7 @@
         <v>43222.3958333335</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>43222.4027777779</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1980,7 @@
         <v>43222.4097222224</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1989,7 @@
         <v>43222.4166666668</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +1998,7 @@
         <v>43222.4236111113</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,7 +2007,7 @@
         <v>43222.4305555557</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2016,7 @@
         <v>43222.4375000002</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2025,7 @@
         <v>43222.4444444446</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2034,7 @@
         <v>43222.4513888891</v>
       </c>
       <c r="B211" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2043,7 @@
         <v>43222.4583333335</v>
       </c>
       <c r="B212" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,7 +2052,7 @@
         <v>43222.4652777779</v>
       </c>
       <c r="B213" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2061,7 @@
         <v>43222.4722222224</v>
       </c>
       <c r="B214" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>43222.4791666668</v>
       </c>
       <c r="B215" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2079,7 @@
         <v>43222.4861111113</v>
       </c>
       <c r="B216" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2088,7 @@
         <v>43222.4930555557</v>
       </c>
       <c r="B217" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,7 +2097,7 @@
         <v>43222.5000000002</v>
       </c>
       <c r="B218" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2106,7 @@
         <v>43222.5069444446</v>
       </c>
       <c r="B219" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +2115,7 @@
         <v>43222.5138888891</v>
       </c>
       <c r="B220" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2124,7 @@
         <v>43222.5208333335</v>
       </c>
       <c r="B221" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2133,7 @@
         <v>43222.527777778</v>
       </c>
       <c r="B222" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2142,7 @@
         <v>43222.5347222224</v>
       </c>
       <c r="B223" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,7 +2151,7 @@
         <v>43222.5416666669</v>
       </c>
       <c r="B224" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>43222.5486111113</v>
       </c>
       <c r="B225" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2169,7 @@
         <v>43222.5555555557</v>
       </c>
       <c r="B226" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2178,7 @@
         <v>43222.5625000002</v>
       </c>
       <c r="B227" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2187,7 @@
         <v>43222.5694444446</v>
       </c>
       <c r="B228" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2196,7 @@
         <v>43222.5763888891</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2205,7 @@
         <v>43222.5833333335</v>
       </c>
       <c r="B230" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,7 +2214,7 @@
         <v>43222.590277778</v>
       </c>
       <c r="B231" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2223,7 @@
         <v>43222.5972222224</v>
       </c>
       <c r="B232" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2232,7 @@
         <v>43222.6041666669</v>
       </c>
       <c r="B233" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,7 +2241,7 @@
         <v>43222.6111111113</v>
       </c>
       <c r="B234" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2250,7 @@
         <v>43222.6180555557</v>
       </c>
       <c r="B235" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,7 +2259,7 @@
         <v>43222.6250000002</v>
       </c>
       <c r="B236" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2268,7 @@
         <v>43222.6319444446</v>
       </c>
       <c r="B237" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2277,7 @@
         <v>43222.6388888891</v>
       </c>
       <c r="B238" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>43222.6458333335</v>
       </c>
       <c r="B239" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,7 +2295,7 @@
         <v>43222.652777778</v>
       </c>
       <c r="B240" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,7 +2304,7 @@
         <v>43222.6597222224</v>
       </c>
       <c r="B241" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2313,7 @@
         <v>43222.6666666669</v>
       </c>
       <c r="B242" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2322,7 @@
         <v>43222.6736111113</v>
       </c>
       <c r="B243" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,7 +2331,7 @@
         <v>43222.6805555558</v>
       </c>
       <c r="B244" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2340,7 @@
         <v>43222.6875000002</v>
       </c>
       <c r="B245" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2349,7 @@
         <v>43222.6944444446</v>
       </c>
       <c r="B246" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,7 +2358,7 @@
         <v>43222.7013888891</v>
       </c>
       <c r="B247" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,7 +2367,7 @@
         <v>43222.7083333335</v>
       </c>
       <c r="B248" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,7 +2376,7 @@
         <v>43222.715277778</v>
       </c>
       <c r="B249" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>43222.7222222224</v>
       </c>
       <c r="B250" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2394,7 @@
         <v>43222.7291666669</v>
       </c>
       <c r="B251" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2403,7 @@
         <v>43222.7361111113</v>
       </c>
       <c r="B252" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,7 +2412,7 @@
         <v>43222.7430555558</v>
       </c>
       <c r="B253" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2421,7 @@
         <v>43222.7500000002</v>
       </c>
       <c r="B254" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2430,7 @@
         <v>43222.7569444447</v>
       </c>
       <c r="B255" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,7 +2439,7 @@
         <v>43222.7638888891</v>
       </c>
       <c r="B256" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,7 +2448,7 @@
         <v>43222.7708333335</v>
       </c>
       <c r="B257" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2457,7 @@
         <v>43222.777777778</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2466,7 @@
         <v>43222.7847222224</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2475,7 @@
         <v>43222.7916666669</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>43222.7986111113</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2493,7 @@
         <v>43222.8055555558</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2502,7 @@
         <v>43222.8125000002</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,7 +2511,7 @@
         <v>43222.8194444447</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2520,7 @@
         <v>43222.8263888891</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,7 +2529,7 @@
         <v>43222.8333333335</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,7 +2538,7 @@
         <v>43222.840277778</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2547,7 @@
         <v>43222.8472222224</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,7 +2556,7 @@
         <v>43222.8541666669</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2565,7 @@
         <v>43222.8611111113</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,7 +2574,7 @@
         <v>43222.8680555558</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>43222.8750000002</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2592,7 @@
         <v>43222.8819444447</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,7 +2601,7 @@
         <v>43222.8888888891</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2610,7 @@
         <v>43222.8958333336</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2619,7 @@
         <v>43222.902777778</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,7 +2628,7 @@
         <v>43222.9097222225</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>